<commit_message>
include consecutive shifts to solve schedule
</commit_message>
<xml_diff>
--- a/data/elm_winter_2022/solutions/solution.xlsx
+++ b/data/elm_winter_2022/solutions/solution.xlsx
@@ -488,7 +488,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -530,7 +530,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -782,7 +782,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -908,7 +908,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
@@ -950,7 +950,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -1118,7 +1118,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1160,7 +1160,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -1202,7 +1202,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
@@ -1328,7 +1328,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1412,7 +1412,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Vivian</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1454,7 +1454,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Vivian</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -1496,7 +1496,7 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Noah Williams</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1538,7 +1538,7 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Noah Williams</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1580,7 +1580,7 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -1622,7 +1622,7 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
@@ -1664,7 +1664,7 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1706,7 +1706,7 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1790,7 +1790,7 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1958,7 +1958,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -2000,7 +2000,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Noah Williams</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -2042,7 +2042,7 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -2168,7 +2168,7 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -2252,7 +2252,7 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Vivian</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -2294,7 +2294,7 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -2336,7 +2336,7 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Vivian</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -2378,7 +2378,7 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Vivian</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
@@ -2462,7 +2462,7 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Noah Williams</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2504,7 +2504,7 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2672,7 +2672,7 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2756,7 +2756,7 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Vivian</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Vivian</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2840,7 +2840,7 @@
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Noah Williams</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2882,7 +2882,7 @@
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Noah Williams</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -3092,7 +3092,7 @@
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Vivian</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -3134,7 +3134,7 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Noah Williams</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -3176,7 +3176,7 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
@@ -3260,7 +3260,7 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -3302,7 +3302,7 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -3428,7 +3428,7 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -3512,7 +3512,7 @@
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Noah Williams</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -3554,7 +3554,7 @@
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Noah Williams</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -3596,7 +3596,7 @@
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Vivian</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3638,7 +3638,7 @@
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Vivian</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3680,7 +3680,7 @@
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Vivian</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3722,7 +3722,7 @@
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Vivian</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
@@ -3806,7 +3806,7 @@
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Noah Williams</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3848,7 +3848,7 @@
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3890,7 +3890,7 @@
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Vivian</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
@@ -4016,7 +4016,7 @@
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -4142,7 +4142,7 @@
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -4184,7 +4184,7 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>Noah Williams</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D90" t="inlineStr">
@@ -4226,7 +4226,7 @@
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Noah Williams</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -4268,7 +4268,7 @@
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
@@ -4310,7 +4310,7 @@
       </c>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
@@ -4352,7 +4352,7 @@
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -4394,7 +4394,7 @@
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -4478,7 +4478,7 @@
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -4520,7 +4520,7 @@
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -4562,7 +4562,7 @@
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -4604,7 +4604,7 @@
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -4646,7 +4646,7 @@
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -4688,7 +4688,7 @@
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
@@ -4730,7 +4730,7 @@
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Vivian</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
@@ -4772,7 +4772,7 @@
       </c>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Vivian</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
@@ -4814,7 +4814,7 @@
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Vivian</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -4898,7 +4898,7 @@
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Noah Williams</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -5108,7 +5108,7 @@
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -5192,7 +5192,7 @@
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
@@ -5276,7 +5276,7 @@
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -5318,7 +5318,7 @@
       </c>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -5360,7 +5360,7 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -5402,7 +5402,7 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Vivian</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
@@ -5444,7 +5444,7 @@
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Vivian</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -5486,7 +5486,7 @@
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Vivian</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
@@ -5528,7 +5528,7 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
@@ -5654,7 +5654,7 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Noah Williams</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -5780,7 +5780,7 @@
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Noah Williams</t>
+          <t>Vivian</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
@@ -5822,7 +5822,7 @@
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -5864,7 +5864,7 @@
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D130" t="inlineStr">
@@ -5906,7 +5906,7 @@
       </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Noah Williams</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
@@ -6032,7 +6032,7 @@
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
@@ -6074,7 +6074,7 @@
       </c>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -6200,7 +6200,7 @@
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Noah Williams</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -6242,7 +6242,7 @@
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Noah Williams</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -6284,7 +6284,7 @@
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
@@ -6326,7 +6326,7 @@
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D141" t="inlineStr">
@@ -6368,7 +6368,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
@@ -6410,7 +6410,7 @@
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Owen Nevaril</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D143" t="inlineStr">
@@ -6494,7 +6494,7 @@
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Natalie O'Rourke</t>
         </is>
       </c>
       <c r="D145" t="inlineStr">
@@ -6536,7 +6536,7 @@
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Natalie O'Rourke</t>
+          <t>Justyna Swierz</t>
         </is>
       </c>
       <c r="D146" t="inlineStr">
@@ -6578,7 +6578,7 @@
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Noah Williams</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D147" t="inlineStr">
@@ -6620,7 +6620,7 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Alexander Betz</t>
+          <t>Aspen</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
@@ -6662,7 +6662,7 @@
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Aspen</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D149" t="inlineStr">
@@ -6704,7 +6704,7 @@
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Noah Williams</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
@@ -6746,7 +6746,7 @@
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Justyna Swierz</t>
+          <t>Tran Nguyen</t>
         </is>
       </c>
       <c r="D151" t="inlineStr">
@@ -6788,7 +6788,7 @@
       </c>
       <c r="C152" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Owen Nevaril</t>
         </is>
       </c>
       <c r="D152" t="inlineStr">
@@ -6914,7 +6914,7 @@
       </c>
       <c r="C155" t="inlineStr">
         <is>
-          <t>Tran Nguyen</t>
+          <t>Alexander Betz</t>
         </is>
       </c>
       <c r="D155" t="inlineStr">

</xml_diff>